<commit_message>
Update RS of MS-OXWSFOLD according to the document of v20181001
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C55193-3990-497E-8CD9-3CB77A33D50D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -21,8 +22,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpC091" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpC091" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-yahan.FAREAST\AppData\Local\Temp\tmpC091.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1180,9 +1181,6 @@
   </si>
   <si>
     <t>Web Service Item ID Algorithm</t>
-  </si>
-  <si>
-    <t>1.0</t>
   </si>
   <si>
     <t>[In Compression Type (byte)] Otherwise [the compressed Id is greater than or equal to the uncompressed Id], the value of this byte [Compression Type] is 0, indicating that no compressions was used.</t>
@@ -1281,20 +1279,23 @@
       <t>: Indicates that a requirement is verified when deserializing the response message.</t>
     </r>
   </si>
+  <si>
+    <t>3.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1337,7 +1338,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1497,7 +1498,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1506,7 +1507,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1539,7 +1540,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1599,7 +1600,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
     <dxf>
@@ -2143,34 +2144,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I82" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I82" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I82" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2179,19 +2180,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2266,6 +2267,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2301,6 +2319,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2476,27 +2511,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>171</v>
       </c>
@@ -2506,7 +2543,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
         <v>172</v>
       </c>
@@ -2517,22 +2554,22 @@
       <c r="F2" s="26"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13">
-        <v>42093</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="21">
       <c r="A4" s="33" t="s">
         <v>18</v>
       </c>
@@ -2544,7 +2581,7 @@
       <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
@@ -2560,7 +2597,7 @@
       <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
@@ -2576,7 +2613,7 @@
       <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
@@ -2592,7 +2629,7 @@
       <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
@@ -2608,7 +2645,7 @@
       <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
@@ -2624,7 +2661,7 @@
       <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
@@ -2640,7 +2677,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
@@ -2656,7 +2693,7 @@
       <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
@@ -2674,7 +2711,7 @@
       <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="28" t="s">
         <v>6</v>
       </c>
@@ -2692,7 +2729,7 @@
       <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
@@ -2710,7 +2747,7 @@
       <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="29" t="s">
         <v>3</v>
       </c>
@@ -2728,7 +2765,7 @@
       <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
@@ -2744,12 +2781,12 @@
       <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="80.25" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
@@ -2760,7 +2797,7 @@
       <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
@@ -2777,7 +2814,7 @@
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="27.6" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2807,7 +2844,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="24" customFormat="1" ht="375" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="24" customFormat="1" ht="390">
       <c r="A20" s="23" t="s">
         <v>34</v>
       </c>
@@ -2826,7 +2863,7 @@
       <c r="H20" s="23"/>
       <c r="I20" s="25"/>
     </row>
-    <row r="21" spans="1:12" s="24" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="24" customFormat="1" ht="60">
       <c r="A21" s="23" t="s">
         <v>35</v>
       </c>
@@ -2845,7 +2882,7 @@
       <c r="H21" s="23"/>
       <c r="I21" s="25"/>
     </row>
-    <row r="22" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A22" s="23" t="s">
         <v>36</v>
       </c>
@@ -2864,7 +2901,7 @@
       <c r="H22" s="23"/>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A23" s="23" t="s">
         <v>37</v>
       </c>
@@ -2883,7 +2920,7 @@
       <c r="H23" s="23"/>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:12" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A24" s="23" t="s">
         <v>38</v>
       </c>
@@ -2902,7 +2939,7 @@
       <c r="H24" s="23"/>
       <c r="I24" s="25"/>
     </row>
-    <row r="25" spans="1:12" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A25" s="23" t="s">
         <v>39</v>
       </c>
@@ -2921,7 +2958,7 @@
       <c r="H25" s="23"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="1:12" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A26" s="23" t="s">
         <v>40</v>
       </c>
@@ -2940,7 +2977,7 @@
       <c r="H26" s="23"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A27" s="23" t="s">
         <v>41</v>
       </c>
@@ -2959,7 +2996,7 @@
       <c r="H27" s="23"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A28" s="23" t="s">
         <v>42</v>
       </c>
@@ -2978,7 +3015,7 @@
       <c r="H28" s="23"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A29" s="23" t="s">
         <v>43</v>
       </c>
@@ -2997,7 +3034,7 @@
       <c r="H29" s="23"/>
       <c r="I29" s="25"/>
     </row>
-    <row r="30" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A30" s="23" t="s">
         <v>44</v>
       </c>
@@ -3016,7 +3053,7 @@
       <c r="H30" s="23"/>
       <c r="I30" s="25"/>
     </row>
-    <row r="31" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="24" customFormat="1" ht="30">
       <c r="A31" s="23" t="s">
         <v>45</v>
       </c>
@@ -3035,7 +3072,7 @@
       <c r="H31" s="23"/>
       <c r="I31" s="25"/>
     </row>
-    <row r="32" spans="1:12" s="24" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="24" customFormat="1" ht="45">
       <c r="A32" s="23" t="s">
         <v>46</v>
       </c>
@@ -3054,7 +3091,7 @@
       <c r="H32" s="23"/>
       <c r="I32" s="25"/>
     </row>
-    <row r="33" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="24" customFormat="1" ht="30">
       <c r="A33" s="23" t="s">
         <v>47</v>
       </c>
@@ -3073,7 +3110,7 @@
       <c r="H33" s="23"/>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30">
       <c r="A34" s="30" t="s">
         <v>48</v>
       </c>
@@ -3092,7 +3129,7 @@
       <c r="H34" s="30"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="45">
       <c r="A35" s="30" t="s">
         <v>49</v>
       </c>
@@ -3111,7 +3148,7 @@
       <c r="H35" s="30"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="30" t="s">
         <v>50</v>
       </c>
@@ -3130,7 +3167,7 @@
       <c r="H36" s="30"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="45">
       <c r="A37" s="30" t="s">
         <v>51</v>
       </c>
@@ -3138,7 +3175,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
@@ -3149,7 +3186,7 @@
       <c r="H37" s="30"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="30" t="s">
         <v>52</v>
       </c>
@@ -3168,7 +3205,7 @@
       <c r="H38" s="30"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="409.5">
       <c r="A39" s="30" t="s">
         <v>53</v>
       </c>
@@ -3187,7 +3224,7 @@
       <c r="H39" s="30"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="409.5">
       <c r="A40" s="30" t="s">
         <v>54</v>
       </c>
@@ -3206,7 +3243,7 @@
       <c r="H40" s="30"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="30" t="s">
         <v>55</v>
       </c>
@@ -3225,7 +3262,7 @@
       <c r="H41" s="30"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="409.5">
       <c r="A42" s="30" t="s">
         <v>56</v>
       </c>
@@ -3244,7 +3281,7 @@
       <c r="H42" s="30"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="409.5">
       <c r="A43" s="30" t="s">
         <v>57</v>
       </c>
@@ -3263,7 +3300,7 @@
       <c r="H43" s="30"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="409.5">
       <c r="A44" s="30" t="s">
         <v>58</v>
       </c>
@@ -3282,7 +3319,7 @@
       <c r="H44" s="30"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="409.5">
       <c r="A45" s="30" t="s">
         <v>59</v>
       </c>
@@ -3301,7 +3338,7 @@
       <c r="H45" s="30"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="409.5">
       <c r="A46" s="30" t="s">
         <v>60</v>
       </c>
@@ -3320,7 +3357,7 @@
       <c r="H46" s="30"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="409.5">
       <c r="A47" s="30" t="s">
         <v>61</v>
       </c>
@@ -3339,7 +3376,7 @@
       <c r="H47" s="30"/>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="30">
       <c r="A48" s="30" t="s">
         <v>62</v>
       </c>
@@ -3358,7 +3395,7 @@
       <c r="H48" s="30"/>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30">
       <c r="A49" s="30" t="s">
         <v>63</v>
       </c>
@@ -3377,7 +3414,7 @@
       <c r="H49" s="30"/>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="330">
       <c r="A50" s="30" t="s">
         <v>64</v>
       </c>
@@ -3396,7 +3433,7 @@
       <c r="H50" s="30"/>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="330">
       <c r="A51" s="30" t="s">
         <v>65</v>
       </c>
@@ -3415,7 +3452,7 @@
       <c r="H51" s="30"/>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="330" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="330">
       <c r="A52" s="30" t="s">
         <v>66</v>
       </c>
@@ -3434,7 +3471,7 @@
       <c r="H52" s="30"/>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="105">
       <c r="A53" s="30" t="s">
         <v>67</v>
       </c>
@@ -3453,7 +3490,7 @@
       <c r="H53" s="30"/>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="75">
       <c r="A54" s="30" t="s">
         <v>68</v>
       </c>
@@ -3472,7 +3509,7 @@
       <c r="H54" s="30"/>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="60">
       <c r="A55" s="30" t="s">
         <v>69</v>
       </c>
@@ -3491,7 +3528,7 @@
       <c r="H55" s="30"/>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="60">
       <c r="A56" s="30" t="s">
         <v>70</v>
       </c>
@@ -3510,7 +3547,7 @@
       <c r="H56" s="30"/>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="60">
       <c r="A57" s="30" t="s">
         <v>71</v>
       </c>
@@ -3529,7 +3566,7 @@
       <c r="H57" s="30"/>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="105">
       <c r="A58" s="30" t="s">
         <v>72</v>
       </c>
@@ -3548,7 +3585,7 @@
       <c r="H58" s="30"/>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="105">
       <c r="A59" s="30" t="s">
         <v>73</v>
       </c>
@@ -3567,7 +3604,7 @@
       <c r="H59" s="30"/>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="75">
       <c r="A60" s="30" t="s">
         <v>74</v>
       </c>
@@ -3586,7 +3623,7 @@
       <c r="H60" s="30"/>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="75">
       <c r="A61" s="30" t="s">
         <v>75</v>
       </c>
@@ -3605,7 +3642,7 @@
       <c r="H61" s="30"/>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="60">
       <c r="A62" s="30" t="s">
         <v>76</v>
       </c>
@@ -3624,7 +3661,7 @@
       <c r="H62" s="30"/>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="75">
       <c r="A63" s="30" t="s">
         <v>77</v>
       </c>
@@ -3643,7 +3680,7 @@
       <c r="H63" s="30"/>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="60">
       <c r="A64" s="30" t="s">
         <v>78</v>
       </c>
@@ -3662,7 +3699,7 @@
       <c r="H64" s="30"/>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="60">
       <c r="A65" s="30" t="s">
         <v>79</v>
       </c>
@@ -3681,7 +3718,7 @@
       <c r="H65" s="30"/>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="45">
       <c r="A66" s="30" t="s">
         <v>80</v>
       </c>
@@ -3700,7 +3737,7 @@
       <c r="H66" s="30"/>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="75">
       <c r="A67" s="30" t="s">
         <v>81</v>
       </c>
@@ -3719,7 +3756,7 @@
       <c r="H67" s="30"/>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="75">
       <c r="A68" s="30" t="s">
         <v>82</v>
       </c>
@@ -3738,7 +3775,7 @@
       <c r="H68" s="30"/>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="105">
       <c r="A69" s="30" t="s">
         <v>83</v>
       </c>
@@ -3757,7 +3794,7 @@
       <c r="H69" s="30"/>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="75">
       <c r="A70" s="30" t="s">
         <v>84</v>
       </c>
@@ -3776,7 +3813,7 @@
       <c r="H70" s="30"/>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="45">
       <c r="A71" s="30" t="s">
         <v>85</v>
       </c>
@@ -3795,7 +3832,7 @@
       <c r="H71" s="30"/>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="45">
       <c r="A72" s="30" t="s">
         <v>86</v>
       </c>
@@ -3814,7 +3851,7 @@
       <c r="H72" s="30"/>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="45">
       <c r="A73" s="30" t="s">
         <v>87</v>
       </c>
@@ -3833,7 +3870,7 @@
       <c r="H73" s="30"/>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="30">
       <c r="A74" s="30" t="s">
         <v>88</v>
       </c>
@@ -3852,7 +3889,7 @@
       <c r="H74" s="30"/>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30">
       <c r="A75" s="30" t="s">
         <v>89</v>
       </c>
@@ -3871,7 +3908,7 @@
       <c r="H75" s="30"/>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9">
       <c r="A76" s="30" t="s">
         <v>90</v>
       </c>
@@ -3890,7 +3927,7 @@
       <c r="H76" s="30"/>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="90">
       <c r="A77" s="30" t="s">
         <v>91</v>
       </c>
@@ -3909,7 +3946,7 @@
       <c r="H77" s="30"/>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="45">
       <c r="A78" s="30" t="s">
         <v>92</v>
       </c>
@@ -3928,7 +3965,7 @@
       <c r="H78" s="30"/>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30">
       <c r="A79" s="30" t="s">
         <v>93</v>
       </c>
@@ -3947,7 +3984,7 @@
       <c r="H79" s="30"/>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="30">
       <c r="A80" s="30" t="s">
         <v>94</v>
       </c>
@@ -3966,7 +4003,7 @@
       <c r="H80" s="30"/>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="30" t="s">
         <v>95</v>
       </c>
@@ -3985,7 +4022,7 @@
       <c r="H81" s="30"/>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="60">
       <c r="A82" s="30" t="s">
         <v>96</v>
       </c>
@@ -4004,11 +4041,11 @@
       <c r="H82" s="30"/>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9">
       <c r="A83" s="3"/>
       <c r="B83" s="10"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9">
       <c r="A84" s="3"/>
       <c r="B84" s="10"/>
     </row>
@@ -4081,20 +4118,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F82" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E82" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G82">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G82" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H82">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H82" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Message Deserialization, Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4104,7 +4141,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B20:B84 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B20:B84" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -4114,12 +4151,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update RS of MS-OXWSITEMID and MS-OXWSFOLD
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C55193-3990-497E-8CD9-3CB77A33D50D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB273CF8-614B-47A7-BCE8-39E33C3C9EDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -1049,14 +1049,6 @@
 Read Int16 from stream for length.
 Read 'length' number of bytes from stream.
 Return as byte[].</t>
-  </si>
-  <si>
-    <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is ConversationIdMailboxGuidBased, the format of the remaining bytes is
-[Short] Moniker Length
-[Variable] Moniker Bytes
-[Byte] Id Processing Instruction (Normal = 0, Recurrence = 1)
-[Short] Store Id Bytes Length
-[Variable] Store Id Bytes</t>
   </si>
   <si>
     <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is MailboxItemMailboxGuidBased&lt;2&gt;, the format of the remaining bytes is
@@ -1281,6 +1273,14 @@
   </si>
   <si>
     <t>3.0</t>
+  </si>
+  <si>
+    <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is ConversationIdMailboxGuidBased, the format of the remaining bytes is
+[Short] Moniker Length
+[Variable] Moniker Bytes
+[Byte] Id Processing Instruction (Normal = 0, Recurrence = 1,Series = 2)
+[Short] Store Id Bytes Length
+[Variable] Store Id Bytes</t>
   </si>
 </sst>
 </file>
@@ -1559,21 +1559,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1597,6 +1582,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2515,8 +2515,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I6"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2535,7 +2535,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2559,7 +2559,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>33</v>
@@ -2570,127 +2570,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2703,12 +2703,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2721,12 +2721,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2739,12 +2739,12 @@
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2757,60 +2757,60 @@
       <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="80.25" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="B17" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3175,7 +3175,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
@@ -3573,8 +3573,8 @@
       <c r="B58" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="32" t="s">
-        <v>146</v>
+      <c r="C58" s="21" t="s">
+        <v>175</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -3593,7 +3593,7 @@
         <v>104</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30"/>
@@ -3612,7 +3612,7 @@
         <v>104</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -3631,7 +3631,7 @@
         <v>104</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30"/>
@@ -3650,7 +3650,7 @@
         <v>104</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -3669,7 +3669,7 @@
         <v>104</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30"/>
@@ -3688,7 +3688,7 @@
         <v>105</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -3707,7 +3707,7 @@
         <v>105</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
@@ -3726,7 +3726,7 @@
         <v>105</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -3745,7 +3745,7 @@
         <v>105</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -3764,7 +3764,7 @@
         <v>105</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -3783,7 +3783,7 @@
         <v>106</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -3802,7 +3802,7 @@
         <v>106</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -3821,7 +3821,7 @@
         <v>106</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -3840,7 +3840,7 @@
         <v>106</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3859,7 +3859,7 @@
         <v>106</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3878,7 +3878,7 @@
         <v>107</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -3897,7 +3897,7 @@
         <v>107</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30"/>
@@ -3916,7 +3916,7 @@
         <v>107</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -3935,7 +3935,7 @@
         <v>107</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3954,7 +3954,7 @@
         <v>108</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -3973,7 +3973,7 @@
         <v>108</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30"/>
@@ -3992,7 +3992,7 @@
         <v>108</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -4011,7 +4011,7 @@
         <v>108</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
@@ -4030,7 +4030,7 @@
         <v>108</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -4051,6 +4051,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -4058,11 +4063,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H82 A34:I82">

</xml_diff>

<commit_message>
update RS of MS-OXWSITEMID and MS-OXWSCORE
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSITEMID/MS-OXWSITEMID_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB273CF8-614B-47A7-BCE8-39E33C3C9EDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3E156-2DF2-40C5-BED8-7DE603299950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,14 +1049,6 @@
 Read Int16 from stream for length.
 Read 'length' number of bytes from stream.
 Return as byte[].</t>
-  </si>
-  <si>
-    <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is MailboxItemMailboxGuidBased&lt;2&gt;, the format of the remaining bytes is
-[Short] Moniker Length
-[Variable] Moniker Bytes
-[Byte] Id Processing Instruction (Normal = 0, Recurrence = 1)
-[Short] Store Id Bytes Length
-[Variable] Store Id Bytes</t>
   </si>
   <si>
     <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] To read these [the remaining bytes] values, perform the following steps.
@@ -1276,6 +1268,14 @@
   </si>
   <si>
     <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is ConversationIdMailboxGuidBased, the format of the remaining bytes is
+[Short] Moniker Length
+[Variable] Moniker Bytes
+[Byte] Id Processing Instruction (Normal = 0, Recurrence = 1,Series = 2)
+[Short] Store Id Bytes Length
+[Variable] Store Id Bytes</t>
+  </si>
+  <si>
+    <t>[In MailboxItemMailboxGuidBased or ConversationIdMailboxGuidBased] If the Id storage type is MailboxItemMailboxGuidBased&lt;2&gt;, the format of the remaining bytes is
 [Short] Moniker Length
 [Variable] Moniker Bytes
 [Byte] Id Processing Instruction (Normal = 0, Recurrence = 1,Series = 2)
@@ -1559,6 +1559,21 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1582,21 +1597,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2515,9 +2515,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -2535,7 +2533,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -2545,7 +2543,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2559,7 +2557,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>33</v>
@@ -2570,127 +2568,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2703,12 +2701,12 @@
       <c r="C12" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2721,12 +2719,12 @@
       <c r="C13" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2739,12 +2737,12 @@
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2757,60 +2755,60 @@
       <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="80.25" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="B17" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3175,7 +3173,7 @@
         <v>99</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
@@ -3574,7 +3572,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30"/>
@@ -3592,8 +3590,8 @@
       <c r="B59" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>146</v>
+      <c r="C59" s="21" t="s">
+        <v>175</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30"/>
@@ -3612,7 +3610,7 @@
         <v>104</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30"/>
@@ -3631,7 +3629,7 @@
         <v>104</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30"/>
@@ -3650,7 +3648,7 @@
         <v>104</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30"/>
@@ -3669,7 +3667,7 @@
         <v>104</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30"/>
@@ -3688,7 +3686,7 @@
         <v>105</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30"/>
@@ -3707,7 +3705,7 @@
         <v>105</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30"/>
@@ -3726,7 +3724,7 @@
         <v>105</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30"/>
@@ -3745,7 +3743,7 @@
         <v>105</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30"/>
@@ -3764,7 +3762,7 @@
         <v>105</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30"/>
@@ -3783,7 +3781,7 @@
         <v>106</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30"/>
@@ -3802,7 +3800,7 @@
         <v>106</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30"/>
@@ -3821,7 +3819,7 @@
         <v>106</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30"/>
@@ -3840,7 +3838,7 @@
         <v>106</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3859,7 +3857,7 @@
         <v>106</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3878,7 +3876,7 @@
         <v>107</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -3897,7 +3895,7 @@
         <v>107</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30"/>
@@ -3916,7 +3914,7 @@
         <v>107</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30"/>
@@ -3935,7 +3933,7 @@
         <v>107</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30"/>
@@ -3954,7 +3952,7 @@
         <v>108</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30"/>
@@ -3973,7 +3971,7 @@
         <v>108</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30"/>
@@ -3992,7 +3990,7 @@
         <v>108</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -4011,7 +4009,7 @@
         <v>108</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
@@ -4030,7 +4028,7 @@
         <v>108</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30"/>
@@ -4051,11 +4049,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -4063,6 +4056,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H82 A34:I82">

</xml_diff>